<commit_message>
T8B - agora em mA :)
</commit_message>
<xml_diff>
--- a/T8B - Frank-Hertz.xlsx
+++ b/T8B - Frank-Hertz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98384A65-64A3-4709-9F71-E13F4EE3BBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33DA450-45DE-4CC9-B019-390115963CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AB49ADD9-0CA5-4C82-AD99-5ED7E5189E9C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Vmin</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>u(I)</t>
+  </si>
+  <si>
+    <t>I (mA)</t>
   </si>
 </sst>
 </file>
@@ -238,9 +241,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,6 +248,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2289,7 +2292,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4464,7 +4467,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5399,7 +5402,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5960,7 +5963,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Resíduos</a:t>
+                  <a:t>Resíduos de I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6717,7 +6720,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" sz="1400"/>
-                  <a:t>Resíduos de I (A)</a:t>
+                  <a:t>Resíduos de I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8200,7 +8203,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10375,7 +10378,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11310,7 +11313,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -14055,7 +14058,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -15544,7 +15547,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>I (A)</a:t>
+                  <a:t>I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -16256,7 +16259,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT" sz="1400"/>
-                  <a:t>Resíduos de I (A)</a:t>
+                  <a:t>Resíduos de I (mA)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -23817,8 +23820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BC4E1F-DE34-448F-AA19-AE0EE9C0CA35}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A5" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23848,7 +23851,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>23</v>
@@ -23903,12 +23906,12 @@
         <f t="shared" si="1"/>
         <v>-0.61250871460386624</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
       <c r="N3" s="9" t="s">
         <v>0</v>
       </c>
@@ -24751,45 +24754,45 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>5.6689999999999996</v>
       </c>
-      <c r="B39" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="C39" s="14">
+      <c r="B39" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="C39" s="13">
         <v>0.26</v>
       </c>
-      <c r="D39" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="E39" s="14">
+      <c r="D39" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E39" s="13">
         <f t="shared" si="2"/>
         <v>0.25360630239826543</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="13">
         <f t="shared" si="3"/>
         <v>6.3936976017345826E-3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="15">
+      <c r="A40" s="14">
         <v>5.7190000000000003</v>
       </c>
-      <c r="B40" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="C40" s="13">
+      <c r="B40" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="C40" s="12">
         <v>0.25700000000000001</v>
       </c>
-      <c r="D40" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="E40" s="13">
+      <c r="D40" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="E40" s="12">
         <f t="shared" si="2"/>
         <v>0.25255448269675707</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="12">
         <f t="shared" si="3"/>
         <v>4.4455173032429407E-3</v>
       </c>
@@ -25930,7 +25933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{373E475D-FABE-447D-A5A2-77A25D8F5E9F}">
   <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:N4"/>
     </sheetView>
   </sheetViews>
@@ -25995,12 +25998,12 @@
         <f>C2-E2</f>
         <v>0.56227565016946346</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
       <c r="M2" s="9" t="s">
         <v>19</v>
       </c>
@@ -27402,45 +27405,45 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>18.899999999999999</v>
       </c>
-      <c r="B64" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="C64" s="14">
+      <c r="B64" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="C64" s="13">
         <v>0.22109999999999999</v>
       </c>
-      <c r="D64" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="E64" s="14">
+      <c r="D64" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E64" s="13">
         <f t="shared" si="0"/>
         <v>0.22101102281376933</v>
       </c>
-      <c r="F64" s="14">
+      <c r="F64" s="13">
         <f t="shared" si="1"/>
         <v>8.8977186230659866E-5</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="15">
+      <c r="A65" s="14">
         <v>19.096</v>
       </c>
-      <c r="B65" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="C65" s="13">
+      <c r="B65" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="C65" s="12">
         <v>0.2286</v>
       </c>
-      <c r="D65" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="E65" s="13">
+      <c r="D65" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="E65" s="12">
         <f t="shared" si="0"/>
         <v>0.22842264494951553</v>
       </c>
-      <c r="F65" s="13">
+      <c r="F65" s="12">
         <f t="shared" si="1"/>
         <v>1.7735505048446787E-4</v>
       </c>
@@ -27833,8 +27836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A6B64E-E440-49D1-98F4-8A1739F15DFD}">
   <dimension ref="B33:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27850,12 +27853,12 @@
   </cols>
   <sheetData>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
       <c r="G33" s="11" t="s">
         <v>0</v>
       </c>
@@ -27883,12 +27886,12 @@
       <c r="H34" s="2">
         <v>0.28505799999999998</v>
       </c>
-      <c r="N34" s="12" t="s">
+      <c r="N34" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
       <c r="S34" s="11" t="s">
         <v>19</v>
       </c>

</xml_diff>